<commit_message>
Responsivitet till ca 500px klar på kategorisida.
</commit_message>
<xml_diff>
--- a/produktbilder/produkter.xlsx
+++ b/produktbilder/produkter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CFdav\Documents\Repos\wp_mockup_webshop\produtbilder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffdb61f3ca5e596b/Gemensamma dokument/3.8. Skolan/WEBB-E-HANDEL/Repos/wp_mockup_webshop/produktbilder/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F4C06A-9762-4874-9CC5-8B1DBFF52EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="-12315" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="2130" windowWidth="15735" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>